<commit_message>
add artigo no template SBC
</commit_message>
<xml_diff>
--- a/Erros a serem corrigidos.xlsx
+++ b/Erros a serem corrigidos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LauraDamacenoDeAlmei\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spaar\Desktop\Artigo Fake News\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0123F79E-09A4-4D0F-B207-76BBE71A78A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7B92EE7-2B4C-4D50-BA45-001D1F5BFB09}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E51FAD2F-C055-4487-886C-47A578C1E8B7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E51FAD2F-C055-4487-886C-47A578C1E8B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="33">
   <si>
     <t>Erros apontados</t>
   </si>
@@ -110,9 +110,6 @@
     <t>Responsável</t>
   </si>
   <si>
-    <t>A ser discutido</t>
-  </si>
-  <si>
     <t>Resolvido</t>
   </si>
   <si>
@@ -129,6 +126,12 @@
   </si>
   <si>
     <t>Acho que resolvi</t>
+  </si>
+  <si>
+    <t>Não será mexida</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -231,7 +234,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -530,16 +533,16 @@
   <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="64.44140625" customWidth="1"/>
-    <col min="2" max="3" width="18.33203125" customWidth="1"/>
+    <col min="1" max="1" width="64.42578125" customWidth="1"/>
+    <col min="2" max="3" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -550,277 +553,285 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C2" s="5"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-    </row>
-    <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="121.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="121.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
     </row>
-    <row r="12" spans="1:3" ht="105.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B23" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
novos ajustes a serem implementados
+ alguns ajustes realizados
</commit_message>
<xml_diff>
--- a/Erros a serem corrigidos.xlsx
+++ b/Erros a serem corrigidos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spaar\Desktop\Artigo Fake News\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LauraDamacenoDeAlmei\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7B92EE7-2B4C-4D50-BA45-001D1F5BFB09}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C74E3919-0396-4D31-A286-B25B6DFA1B37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E51FAD2F-C055-4487-886C-47A578C1E8B7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E51FAD2F-C055-4487-886C-47A578C1E8B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="39">
   <si>
     <t>Erros apontados</t>
   </si>
@@ -132,6 +132,28 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>A equação (2) está incorreta</t>
+  </si>
+  <si>
+    <t>A legenda da Figura 4 contradiz o que há no texto.</t>
+  </si>
+  <si>
+    <t>A Tabela 4 não existe</t>
+  </si>
+  <si>
+    <t>Na hipótese H0 o que são resultados insuficientes?</t>
+  </si>
+  <si>
+    <t>A Tabela 1 não é citada no texto!</t>
+  </si>
+  <si>
+    <t>Corrigir expressões estranhas/Typos: 
+  - notçias
+  - por etapas por um conjunto de etapas
+  - De acordo com a Figura. 3. É possível notar
+  - e, além facilitar a</t>
   </si>
 </sst>
 </file>
@@ -234,7 +256,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -532,17 +554,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B35F130-2E1E-45B8-A465-C306162D50AE}">
   <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="64.42578125" customWidth="1"/>
-    <col min="2" max="3" width="18.28515625" customWidth="1"/>
+    <col min="1" max="1" width="64.44140625" customWidth="1"/>
+    <col min="2" max="3" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -553,7 +575,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -562,7 +584,7 @@
       </c>
       <c r="C2" s="5"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -573,7 +595,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -584,7 +606,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -595,7 +617,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
@@ -606,7 +628,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -617,7 +639,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
@@ -628,7 +650,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -639,7 +661,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
@@ -650,14 +672,14 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="121.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="121.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
     </row>
-    <row r="12" spans="1:3" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="105.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>12</v>
       </c>
@@ -668,7 +690,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>13</v>
       </c>
@@ -679,7 +701,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>14</v>
       </c>
@@ -690,7 +712,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>15</v>
       </c>
@@ -701,7 +723,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>16</v>
       </c>
@@ -712,7 +734,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>17</v>
       </c>
@@ -723,7 +745,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>18</v>
       </c>
@@ -734,7 +756,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>19</v>
       </c>
@@ -745,7 +767,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>20</v>
       </c>
@@ -756,7 +778,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>21</v>
       </c>
@@ -767,7 +789,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>22</v>
       </c>
@@ -778,7 +800,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>23</v>
       </c>
@@ -789,49 +811,81 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+    </row>
+    <row r="29" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ajustes a serem realizados
</commit_message>
<xml_diff>
--- a/Erros a serem corrigidos.xlsx
+++ b/Erros a serem corrigidos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LauraDamacenoDeAlmei\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C74E3919-0396-4D31-A286-B25B6DFA1B37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02A52367-A062-4C01-8DF7-CC46C36A97AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E51FAD2F-C055-4487-886C-47A578C1E8B7}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="54">
   <si>
     <t>Erros apontados</t>
   </si>
@@ -154,6 +154,65 @@
   - por etapas por um conjunto de etapas
   - De acordo com a Figura. 3. É possível notar
   - e, além facilitar a</t>
+  </si>
+  <si>
+    <t>A Seção de Introdução está muito extensa, sem foco e não apresenta elementos fundamentais de uma introdução de artigo. Nela, não fica claro o problema exato que o artigo pretende resolver, como pretende resolver, como os resultados foram avaliados e quais são os resultados gerais</t>
+  </si>
+  <si>
+    <t>Além disto, no último parágrafo deveria haver um sumário das seções posteriores.</t>
+  </si>
+  <si>
+    <t>No geral, além de uma melhor estruturação do texto, o artigo precisa de uma revisão gramatical. Há muitas frases longas, uso incorreto de vírgulas e "emendas" ou "quebras" de frases que comprometem a compreensão do texto.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As conclusões da Seção 5 também são vagas, e não discutem potenciais ameaças a validade dos resultados. Por exemplo, quão dependentes os resultados são do dataset utilizado e das técnicas de limpeza, por exemplo? O texto diz que o artigo apresentou resultados contrários ao apresentado por Dias (2019) em virtude da limpeza dos dados, mas como isto está representado nos resultados? Quais métricas e cenários foram avaliados para que tal conclusão seja obtida? </t>
+  </si>
+  <si>
+    <t>O artigo necessita de uma revisão de português por algumas frases parecerem faltar a completude do raciocínio como por exemplo as seguintes frases:  
+Exemplo1: De acordo com Zhou et al (2020) e outras obras utilizadas como base para o projeto de Monteiro et al (2018) e Shu et al (2017), existem alguns atributos que fazem a ponte entre a exatidão dos modelos de detecção de notícias falsas, tais como: número de palavras, número de pontos, número de parágrafos etc.
+Exemplo 2:  Métodos probabilísticos bayesianos assumem que a probabilidade de um evento A, representado por uma variável alvo, como por exemplo, a classe falsa, dado um evento B, representado por valores de atributos de entrada [Freire e Goldschimidt 2019], por exemplo: as representações numéricas da notícia
+Exemplo 3: - repetição da palavra etapas -  Os dados passaram por etapas por um conjunto de etapas de pré-processamento (ver Figura 2), vetorização, treinamento nos algoritmos de classificação SVM e Naive Bayes (ver Figura 3) e avaliação final que incluíram o cálculo do F1 Score, curva ROC, acurácia e Área Sob a Curva (AUC).</t>
+  </si>
+  <si>
+    <t>Falta de complementos necessariamente baseadas notícias reais  faltando EM
+Na seção Trabalhos Correlatos não são apresentados de forma abrangente trabalhos que tenham buscado responder a mesma pergunta de pesquisa ou até semelhante, com outras técnicas ou maneiras diferentes. Há uma mistura de comparação com alguns trabalhos , mas também com uma parte conceitual. Isso faz com que esta seção esteja mais semelhante a um Referencial teórico do que Trabalhos correlatos.</t>
+  </si>
+  <si>
+    <t>Quanto aos dados utilizados para validação é importante que os autores expliquem se de fato TODAS as notícias veiculadas pelos sites contraponto.jor.br e conversaafiada.com.br/politica são falsas ou se isso é apenas senso comum.</t>
+  </si>
+  <si>
+    <t>Na seção Análise dos Dados, algums discussões são difíceis de acompanhar. Por exemplo  Durante a análise feita na base de treinamento, verificou-se que mais de 75% das notícias falsas têm menos de 218 caracteres de palavras, então notícias falsas tendem a ser mais curtas se comparadas com as não falsas e mais de 75% das notícias não falsas tem número de palavras menor que 1369 caracteres.- fica confuso entender, da forma como está escrito uma mensagem com 100 caracteres se encaixa tanto na explicação de notícias falsas quanto não falsas, pois 100 é menor que 218 e menor que 1369.</t>
+  </si>
+  <si>
+    <t>Figura 6: aumentar a figura para possibilitar a visualização dos dados dos eixos e legendas.</t>
+  </si>
+  <si>
+    <t>Do 5.o parágrafo da Seção 2 em diante poderia ser colocado em uma Seção de "Processamento de Linguagem Natural". Esse conteúdo não está relacionado aos "Trabalhos Correlados" e sim aos conceitos de PLN.</t>
+  </si>
+  <si>
+    <t>Na Seção 3.1, "foram mapeados dois sites que compartilham notícias falsas e dois sites considerados confiáveis...de acordo com a justificativa...". Qual é essa justificativa? Não ficou claro no texto.</t>
+  </si>
+  <si>
+    <t>No Resumo:
+- a versão em inglês diz que o propósito do trabalho é analisar se as notícias políticas são verdadeiras ou não e difere do resumo em português.
+- já no resumo talvez fosse necessário explicar melhor o que é "melhor" resultado.</t>
+  </si>
+  <si>
+    <t>Na Introdução
+- não é feita, claramente, uma menção ao propósito principal do trabalho que é a comparação dos dois algoritmos.
+- a Introdução não dá o suporte que o restante do texto precisa para chegar às conclusões esperadas.</t>
+  </si>
+  <si>
+    <t>Nos Trabalhos Correlatos
+- essa seção não trata de Trabalhos Correlatos, mas, de fundamentação da proposta.
+- há uma discussão sobre a representação das notícias falsas, mas, não se explica o porquê dessa discussão ser necessária.
+- há termos não explicados, tais como stop words
+- o parágrafo que inicia com a frase "O Naive Bayes é um classificador probabilístico que assume a independência entre os atributos dos dados [Harrison 2019]." não possui sentido.</t>
+  </si>
+  <si>
+    <t>Na Metodologia
+- não há claramente explicado o que é um resultado "melhor". Essa explicação já deveria ter sido apresentada nesse ponto.
+- como se chegou ao processo para o pré-processamento das notícias. Esse caminho é muito importante para que se compreenda o que dos trabalhos correlatos temos de adaptação/melhoria/inovação.</t>
   </si>
 </sst>
 </file>
@@ -220,11 +279,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -552,10 +608,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B35F130-2E1E-45B8-A465-C306162D50AE}">
-  <dimension ref="A1:C38"/>
+  <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -565,328 +621,420 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="5"/>
+      <c r="C2" s="4"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="5" t="s">
+      <c r="B3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="5" t="s">
+      <c r="B4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="6" t="s">
+      <c r="B5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="6" t="s">
+      <c r="B7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="5" t="s">
+      <c r="B8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="5" t="s">
+      <c r="B9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="72" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="5" t="s">
+      <c r="B10" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="121.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
     </row>
     <row r="12" spans="1:3" ht="105.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="5" t="s">
+      <c r="B12" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="5" t="s">
+      <c r="B13" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" s="5" t="s">
+      <c r="B15" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" s="5" t="s">
+      <c r="B16" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" s="5" t="s">
+      <c r="B17" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="5" t="s">
+      <c r="B18" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" s="5" t="s">
+      <c r="B19" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C20" s="5" t="s">
+      <c r="B20" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C21" s="5" t="s">
+      <c r="B21" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="4" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="4" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5" t="s">
+      <c r="B24" s="4"/>
+      <c r="C24" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C25" s="5" t="s">
+      <c r="B25" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5" t="s">
+      <c r="B26" s="4"/>
+      <c r="C26" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
     </row>
     <row r="29" spans="1:3" ht="72" x14ac:dyDescent="0.3">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="1"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="1"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="1"/>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" s="1"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" s="1"/>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" s="1"/>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" s="1"/>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A37" s="1"/>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A38" s="1"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+    </row>
+    <row r="30" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+    </row>
+    <row r="31" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+    </row>
+    <row r="32" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+    </row>
+    <row r="33" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+    </row>
+    <row r="34" spans="1:3" ht="259.2" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+    </row>
+    <row r="35" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+    </row>
+    <row r="36" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+    </row>
+    <row r="37" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+    </row>
+    <row r="40" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+    </row>
+    <row r="41" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A41" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B41" s="4"/>
+      <c r="C41" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A42" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
+    </row>
+    <row r="43" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A43" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+    </row>
+    <row r="44" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A44" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="2"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
erros a serem corrigidos
</commit_message>
<xml_diff>
--- a/Erros a serem corrigidos.xlsx
+++ b/Erros a serem corrigidos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LauraDamacenoDeAlmei\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02A52367-A062-4C01-8DF7-CC46C36A97AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED8A3C85-CE32-447B-9897-E7826C0C1EE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E51FAD2F-C055-4487-886C-47A578C1E8B7}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="55">
   <si>
     <t>Erros apontados</t>
   </si>
@@ -213,6 +213,9 @@
     <t>Na Metodologia
 - não há claramente explicado o que é um resultado "melhor". Essa explicação já deveria ter sido apresentada nesse ponto.
 - como se chegou ao processo para o pré-processamento das notícias. Esse caminho é muito importante para que se compreenda o que dos trabalhos correlatos temos de adaptação/melhoria/inovação.</t>
+  </si>
+  <si>
+    <t>A tabela está no artigo</t>
   </si>
 </sst>
 </file>
@@ -608,10 +611,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B35F130-2E1E-45B8-A465-C306162D50AE}">
-  <dimension ref="A1:C46"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -790,7 +793,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>17</v>
       </c>
@@ -801,7 +804,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>18</v>
       </c>
@@ -812,7 +815,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>19</v>
       </c>
@@ -823,7 +826,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>20</v>
       </c>
@@ -834,7 +837,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>21</v>
       </c>
@@ -845,7 +848,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>22</v>
       </c>
@@ -856,7 +859,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>23</v>
       </c>
@@ -867,16 +870,18 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B24" s="4"/>
+      <c r="B24" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="C24" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>34</v>
       </c>
@@ -887,51 +892,58 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B26" s="4"/>
+      <c r="B26" s="4" t="s">
+        <v>32</v>
+      </c>
       <c r="C26" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D26" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
-        <v>37</v>
       </c>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
     </row>
-    <row r="29" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
     </row>
-    <row r="30" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
     </row>
-    <row r="31" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
     </row>
-    <row r="32" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>41</v>
       </c>
@@ -979,7 +991,9 @@
       <c r="A38" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B38" s="4"/>
+      <c r="B38" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="C38" s="4" t="s">
         <v>27</v>
       </c>
@@ -1002,7 +1016,9 @@
       <c r="A41" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B41" s="4"/>
+      <c r="B41" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="C41" s="4" t="s">
         <v>27</v>
       </c>

</xml_diff>

<commit_message>
ajuste de alguns erros - Laura
</commit_message>
<xml_diff>
--- a/Erros a serem corrigidos.xlsx
+++ b/Erros a serem corrigidos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LauraDamacenoDeAlmei\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCCB47C5-C35D-4489-8A60-442369ACB840}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31A06555-638F-4A94-92E9-C7FD0E06E6A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E51FAD2F-C055-4487-886C-47A578C1E8B7}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="57">
   <si>
     <t>Erros apontados</t>
   </si>
@@ -216,6 +216,12 @@
   </si>
   <si>
     <t>A tabela está no artigo</t>
+  </si>
+  <si>
+    <t>Retirei o parágrafo</t>
+  </si>
+  <si>
+    <t>Adicionar a etapa de teste e validação no diagrama da Figura 3</t>
   </si>
 </sst>
 </file>
@@ -613,8 +619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B35F130-2E1E-45B8-A465-C306162D50AE}">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -910,7 +916,9 @@
       <c r="A27" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B27" s="4"/>
+      <c r="B27" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="C27" s="4" t="s">
         <v>27</v>
       </c>
@@ -950,44 +958,49 @@
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
     </row>
-    <row r="33" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
     </row>
-    <row r="34" spans="1:3" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
     </row>
-    <row r="35" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
     </row>
-    <row r="36" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
     </row>
-    <row r="37" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B37" s="4"/>
+      <c r="B37" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="C37" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D37" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>47</v>
       </c>
@@ -998,21 +1011,21 @@
         <v>27</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>48</v>
       </c>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
     </row>
-    <row r="40" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
     </row>
-    <row r="41" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>50</v>
       </c>
@@ -1023,33 +1036,37 @@
         <v>27</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
     </row>
-    <row r="43" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
     </row>
-    <row r="44" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45" s="2"/>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="B45" s="4"/>
-      <c r="C45" s="4"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C45" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ajuste de alguns erros na metodologia e
no diagrama
</commit_message>
<xml_diff>
--- a/Erros a serem corrigidos.xlsx
+++ b/Erros a serem corrigidos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LauraDamacenoDeAlmei\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C812DBD-DE84-4D24-B7A3-052237DF5BD7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05EF245B-BA95-48B5-AF57-89911B843A03}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E51FAD2F-C055-4487-886C-47A578C1E8B7}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="59">
   <si>
     <t>Erros apontados</t>
   </si>
@@ -207,18 +207,28 @@
 - o parágrafo que inicia com a frase "O Naive Bayes é um classificador probabilístico que assume a independência entre os atributos dos dados [Harrison 2019]." não possui sentido.</t>
   </si>
   <si>
+    <t>A tabela está no artigo</t>
+  </si>
+  <si>
+    <t>Retirei o parágrafo</t>
+  </si>
+  <si>
+    <t>Adicionar a etapa de teste e validação no diagrama da Figura 3</t>
+  </si>
+  <si>
     <t>Na Metodologia
-- não há claramente explicado o que é um resultado "melhor". Essa explicação já deveria ter sido apresentada nesse ponto.
-- como se chegou ao processo para o pré-processamento das notícias. Esse caminho é muito importante para que se compreenda o que dos trabalhos correlatos temos de adaptação/melhoria/inovação.</t>
-  </si>
-  <si>
-    <t>A tabela está no artigo</t>
-  </si>
-  <si>
-    <t>Retirei o parágrafo</t>
-  </si>
-  <si>
-    <t>Adicionar a etapa de teste e validação no diagrama da Figura 3</t>
+- não há claramente explicado o que é um resultado "melhor". Essa explicação já deveria ter sido apresentada nesse ponto.</t>
+  </si>
+  <si>
+    <t>Na Metodologia- como se chegou ao processo para o pré-processamento das notícias. Esse caminho é muito importante para que se compreenda o que dos trabalhos correlatos temos de adaptação/melhoria/inovação.</t>
+  </si>
+  <si>
+    <t>acurárica abaixo de 50% (modelo não conseguiu acertar nem 50% dos dados),
+Erro I e II muito altos
+Precisão, recall e F1-Score abaixo de 50%. AUC e curva RoC menor que 50%</t>
+  </si>
+  <si>
+    <t>Definir melhor o que seria um desempenho ruim. (procurar referências)</t>
   </si>
 </sst>
 </file>
@@ -285,7 +295,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -299,6 +309,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -614,16 +627,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B35F130-2E1E-45B8-A465-C306162D50AE}">
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="64.44140625" customWidth="1"/>
     <col min="2" max="3" width="18.33203125" customWidth="1"/>
+    <col min="4" max="4" width="31.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -899,7 +913,7 @@
         <v>26</v>
       </c>
       <c r="D25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -917,8 +931,12 @@
       <c r="A27" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
+      <c r="B27" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="28" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
@@ -987,7 +1005,7 @@
         <v>26</v>
       </c>
       <c r="D36" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -1040,24 +1058,46 @@
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
     </row>
-    <row r="43" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B43" s="4"/>
-      <c r="C43" s="4"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B44" s="4"/>
-      <c r="C44" s="4" t="s">
-        <v>26</v>
-      </c>
+      <c r="C44" s="4"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="2"/>
+      <c r="A45" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A46" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>57</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>